<commit_message>
Changes: Update: Changes in apiService for acopling changes on backend architecture
</commit_message>
<xml_diff>
--- a/ProyectoSmartMed/FuentesSmartMed/incidencias.xlsx
+++ b/ProyectoSmartMed/FuentesSmartMed/incidencias.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documentos\work_projects\medileser\aplicativoSmart\backSmart\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C090A09-1770-407E-8EAF-C0000E10956B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2231794-B823-4EE8-8A2D-C18344C3E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E90C098F-6B10-452D-A8F9-584E2FD75B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="CALLAO AGOSTO" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CALLAO AGOSTO'!$A$1:$K$139</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>TIEMPO DE INCIDENCIA</t>
   </si>
@@ -67,6 +68,66 @@
   </si>
   <si>
     <t>ITEM</t>
+  </si>
+  <si>
+    <t>INCIDENCIAS</t>
+  </si>
+  <si>
+    <t>MEDIDOR MECANICO</t>
+  </si>
+  <si>
+    <t>NIPLE CAJA VACIA</t>
+  </si>
+  <si>
+    <t>NO SE UBICA</t>
+  </si>
+  <si>
+    <t>DIFICIL ACCESO</t>
+  </si>
+  <si>
+    <t>INUNDADO</t>
+  </si>
+  <si>
+    <t>VANDALIZADO</t>
+  </si>
+  <si>
+    <t>DISPLAY APAGADO</t>
+  </si>
+  <si>
+    <t>TEMPERATURA</t>
+  </si>
+  <si>
+    <t>FLUJO INVERSO</t>
+  </si>
+  <si>
+    <t>AIRE EN TUBERIA</t>
+  </si>
+  <si>
+    <t>DIGITOS INCOMPLETOS</t>
+  </si>
+  <si>
+    <t>FUGA DE AGUA</t>
+  </si>
+  <si>
+    <t>FALLO DE FLUJO</t>
+  </si>
+  <si>
+    <t>PROBLEMA DE MEMORIA</t>
+  </si>
+  <si>
+    <t>ESTADO DE COMUNICACION</t>
+  </si>
+  <si>
+    <t>BATERIA BAJA</t>
+  </si>
+  <si>
+    <t>FALLO SENSOR DE TRANSMISION</t>
+  </si>
+  <si>
+    <t>FALLO SENSOR DE TEMPERATURA</t>
+  </si>
+  <si>
+    <t>APERTURA DE TAPA</t>
   </si>
 </sst>
 </file>
@@ -796,7 +857,7 @@
   <dimension ref="A1:K2889"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30181,6 +30242,140 @@
     <cfRule type="duplicateValues" dxfId="1" priority="16"/>
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Por favor ingrese solo fechas" sqref="H1:H1048576" xr:uid="{B2525824-0067-4CAC-935D-C73533328A9F}">
+      <formula1>45292</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Por favor seleccione una de la lista" xr:uid="{E8A38AAB-9339-4C3A-9952-BAE2387836B6}">
+          <x14:formula1>
+            <xm:f>Hoja2!$A$2:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687A9B8B-C5BD-477B-817E-371AAA3056E6}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>